<commit_message>
Updated search results & listing problem
</commit_message>
<xml_diff>
--- a/GooglePlay/SearchResults.xlsx
+++ b/GooglePlay/SearchResults.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Search</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Position</t>
   </si>
@@ -84,7 +81,25 @@
     <t>affiliate</t>
   </si>
   <si>
-    <t>Twitch + …</t>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Search (Twitch + …)</t>
+  </si>
+  <si>
+    <t>1.2.0-a</t>
+  </si>
+  <si>
+    <t>1.2.1-a</t>
+  </si>
+  <si>
+    <t>streamers</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -157,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -199,13 +214,26 @@
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <right/>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -216,15 +244,38 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -530,194 +581,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.140625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
-        <v>43633</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="11">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="11">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="11">
+        <v>29</v>
+      </c>
+      <c r="C15" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="12">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="12">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="11">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="C18" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="11">
+        <v>15</v>
+      </c>
+      <c r="C19" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="11">
+        <v>29</v>
+      </c>
+      <c r="C21" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="11">
+        <v>14</v>
+      </c>
+      <c r="C22" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="7">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="7">
+      <c r="B24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="7">
-        <v>14</v>
-      </c>
-    </row>
+      <c r="B25" s="10">
+        <v>43634</v>
+      </c>
+      <c r="C25" s="10">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Preperation for build 2.1.0-a
</commit_message>
<xml_diff>
--- a/GooglePlay/SearchResults.xlsx
+++ b/GooglePlay/SearchResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cullimoj\StudioProjects\StreamingYorkie\GooglePlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34433CC2-67C5-4637-BB01-DEE69DB6E38A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DF014C-864B-47B0-BB79-4DFE17BFB7FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7935" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>Position</t>
   </si>
@@ -112,6 +112,36 @@
   </si>
   <si>
     <t>partner</t>
+  </si>
+  <si>
+    <t>2.0.3-a</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>chat</t>
+  </si>
+  <si>
+    <t>viewer count</t>
+  </si>
+  <si>
+    <t>bot</t>
+  </si>
+  <si>
+    <t>more viewers</t>
+  </si>
+  <si>
+    <t>discord</t>
+  </si>
+  <si>
+    <t>lurk</t>
+  </si>
+  <si>
+    <t>l4l</t>
   </si>
 </sst>
 </file>
@@ -184,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -236,12 +266,36 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -256,14 +310,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,10 +333,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -630,374 +687,600 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>3</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>5</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>5</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="6">
         <v>16</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>13</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="6">
         <v>28</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>16</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="6">
         <v>29</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>24</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="5">
         <v>5</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>4</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="5">
         <v>6</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>6</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B19" s="6">
         <v>22</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C19" s="6">
         <v>22</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D19" s="6">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="E19" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B20" s="6">
         <v>15</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C20" s="6">
         <v>15</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D20" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="E20" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="6">
+      <c r="B21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="5">
         <v>6</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D21" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="E21" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B22" s="6">
         <v>29</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C22" s="6">
         <v>26</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D22" s="6">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="E22" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B24" s="6">
         <v>14</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C24" s="6">
         <v>14</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D24" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="E24" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="6">
+      <c r="B25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="E25" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="E34" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B35" s="9">
         <v>43634</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C35" s="9">
         <v>43634</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D35" s="9">
         <v>43734</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="E35" s="9">
+        <v>43832</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>